<commit_message>
login path "login" → ""
</commit_message>
<xml_diff>
--- a/web-page-new/src/assets/excel/deviceInsert.xlsx
+++ b/web-page-new/src/assets/excel/deviceInsert.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Han\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1741EA92-809A-4FB8-B3A1-E74E3819CC07}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8FFB11F-C1DF-4D98-A284-20B699D88CE6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-2550" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -125,16 +125,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>SN</t>
-  </si>
-  <si>
     <t>SIMカードICCID</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>SIMカードIMSI</t>
-  </si>
-  <si>
     <t>SIMカード電話番号</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -158,9 +152,6 @@
   </si>
   <si>
     <t>ファームウェア・最新バージョン確認時刻</t>
-  </si>
-  <si>
-    <t>プロダクトID</t>
   </si>
   <si>
     <t>会社ID</t>
@@ -178,13 +169,25 @@
   </si>
   <si>
     <t>元グループID</t>
+  </si>
+  <si>
+    <t>SN</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SIMカードIMSI</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>プロダクトID</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -197,14 +200,6 @@
       <sz val="6"/>
       <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
@@ -231,14 +226,11 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -543,160 +535,162 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="3.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.375" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.75" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="35.375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.75" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="35.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="G2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="L2" t="s">
+      <c r="N2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="P2" t="s">
+      <c r="S2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="T2" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="R2" t="s">
-        <v>37</v>
-      </c>
-      <c r="S2" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>